<commit_message>
Support latest draft of JSF comments/notes types
</commit_message>
<xml_diff>
--- a/tests/excel/comments.xlsx
+++ b/tests/excel/comments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/repos/@flother/xlsx-convert/tests/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/job/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E50E892-9C4B-F64B-A13C-EF6503F72408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D006528-13EE-2B47-A0BA-9EFD0DB60096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{CFBFBE1E-2A86-1D46-AF82-76A77BE0F269}"/>
   </bookViews>
@@ -107,7 +107,9 @@
     It's a comment!
 With some newlines!
 Reply:
-    Love it!</t>
+    Love it!
+Reply:
+    Here's a comment with a link to https://grid.is in the text.</t>
       </text>
     </comment>
   </commentList>
@@ -214,6 +216,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Jón Jónsson" id="{3DB0C038-8ED0-334F-836F-17C97737837B}" userId="Jón Jónsson" providerId="None"/>
+  <person displayName="Jóna Jónsdóttir" id="{8441EF2C-CE6E-0743-B833-FA42010F6747}" userId="Jóna Jónsdóttir" providerId="None"/>
 </personList>
 </file>
 
@@ -541,6 +544,15 @@
   <threadedComment ref="D13" dT="2026-01-26T14:36:28.79" personId="{3DB0C038-8ED0-334F-836F-17C97737837B}" id="{102D4108-9F86-5143-949F-992FEE01EF22}" parentId="{CF327984-011D-6749-8C27-A358EC5BE04A}">
     <text>Love it!</text>
   </threadedComment>
+  <threadedComment ref="D13" dT="2026-01-28T12:31:34.19" personId="{8441EF2C-CE6E-0743-B833-FA42010F6747}" id="{B48EE04D-D9D7-FB43-AC0A-E69F936077C1}" parentId="{CF327984-011D-6749-8C27-A358EC5BE04A}">
+    <text>Here's a comment with a link to https://grid.is in the text.</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3566699083</xltc2:checksum>
+        <xltc2:hyperlink startIndex="32" length="15" url="https://grid.is"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -557,7 +569,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>